<commit_message>
approximate computing exp sim final 3
</commit_message>
<xml_diff>
--- a/unit/exp/software/sim_coeff_select_final_version/sim_coeff_selet_gradient_final_version_summary_uniform.xlsx
+++ b/unit/exp/software/sim_coeff_select_final_version/sim_coeff_selet_gradient_final_version_summary_uniform.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wudidaizi/Project/approximate_computing/unit/exp/software/sim_coeff_select_final_version/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9BA36E0F-1B7B-9442-9AF5-91D10910D655}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{83A3FFA4-21A2-4247-9E9E-DCCE51CEC409}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440"/>
   </bookViews>
@@ -950,7 +950,7 @@
   <dimension ref="A1:AC4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1109,25 +1109,25 @@
         <v>100000000000000</v>
       </c>
       <c r="V2">
-        <v>7.4110999999999996E-2</v>
+        <v>7.4496000000000007E-2</v>
       </c>
       <c r="W2">
-        <v>1.6650999999999999E-2</v>
+        <v>1.7056000000000002E-2</v>
       </c>
       <c r="X2">
-        <v>3.673E-3</v>
+        <v>4.078E-3</v>
       </c>
       <c r="Y2">
-        <v>4.8549999999999999E-3</v>
+        <v>5.2599999999999999E-3</v>
       </c>
       <c r="Z2">
-        <v>2.6459999999999999E-3</v>
+        <v>3.0509999999999999E-3</v>
       </c>
       <c r="AA2">
-        <v>2.2190000000000001E-3</v>
+        <v>2.624E-3</v>
       </c>
       <c r="AB2">
-        <v>2.2190000000000001E-3</v>
+        <v>2.624E-3</v>
       </c>
       <c r="AC2" t="s">
         <v>28</v>
@@ -1198,25 +1198,25 @@
         <v>100000000000000</v>
       </c>
       <c r="V3">
-        <v>0.106227</v>
+        <v>0.10642799999999999</v>
       </c>
       <c r="W3">
-        <v>2.0841999999999999E-2</v>
+        <v>2.0694000000000001E-2</v>
       </c>
       <c r="X3">
-        <v>2.8019999999999998E-3</v>
+        <v>2.6779999999999998E-3</v>
       </c>
       <c r="Y3">
-        <v>3.0140000000000002E-3</v>
+        <v>3.117E-3</v>
       </c>
       <c r="Z3">
-        <v>1.446E-3</v>
+        <v>1.524E-3</v>
       </c>
       <c r="AA3">
-        <v>7.4200000000000004E-4</v>
+        <v>7.9299999999999998E-4</v>
       </c>
       <c r="AB3">
-        <v>4.5600000000000003E-4</v>
+        <v>4.7800000000000002E-4</v>
       </c>
       <c r="AC3" t="s">
         <v>28</v>
@@ -1287,25 +1287,25 @@
         <v>100000000000000</v>
       </c>
       <c r="V4">
-        <v>5.1964000000000003E-2</v>
+        <v>5.1968E-2</v>
       </c>
       <c r="W4">
-        <v>8.6929999999999993E-3</v>
+        <v>8.6910000000000008E-3</v>
       </c>
       <c r="X4">
-        <v>3.0829999999999998E-3</v>
+        <v>3.081E-3</v>
       </c>
       <c r="Y4">
-        <v>1.5039999999999999E-3</v>
+        <v>1.5020000000000001E-3</v>
       </c>
       <c r="Z4">
-        <v>7.1500000000000003E-4</v>
+        <v>7.1400000000000001E-4</v>
       </c>
       <c r="AA4">
-        <v>3.68E-4</v>
+        <v>3.6600000000000001E-4</v>
       </c>
       <c r="AB4">
-        <v>3.68E-4</v>
+        <v>3.6600000000000001E-4</v>
       </c>
       <c r="AC4" t="s">
         <v>28</v>

</xml_diff>